<commit_message>
fix the target bug(didn't check the target the first time)
</commit_message>
<xml_diff>
--- a/Doc/v3/portfolioReturn.xlsx
+++ b/Doc/v3/portfolioReturn.xlsx
@@ -731,7 +731,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-140</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>0</c:v>
@@ -773,10 +773,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -791,31 +791,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-50</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-200</c:v>
+                  <c:v>-160</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-400</c:v>
+                  <c:v>-340</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-800</c:v>
+                  <c:v>-680</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-640</c:v>
+                  <c:v>-520</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-640</c:v>
+                  <c:v>-520</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0</c:v>
@@ -1624,11 +1624,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="198474528"/>
-        <c:axId val="197369016"/>
+        <c:axId val="203945512"/>
+        <c:axId val="256544760"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="198474528"/>
+        <c:axId val="203945512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,14 +1671,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197369016"/>
+        <c:crossAx val="256544760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="197369016"/>
+        <c:axId val="256544760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198474528"/>
+        <c:crossAx val="203945512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2401,7 +2401,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-140</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>0</c:v>
@@ -2443,10 +2443,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -2461,31 +2461,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-50</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-200</c:v>
+                  <c:v>-160</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-200</c:v>
+                  <c:v>-170</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-400</c:v>
+                  <c:v>-340</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-800</c:v>
+                  <c:v>-680</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-640</c:v>
+                  <c:v>-520</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-640</c:v>
+                  <c:v>-520</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0</c:v>
@@ -2582,11 +2582,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="171988656"/>
-        <c:axId val="197803544"/>
+        <c:axId val="256859624"/>
+        <c:axId val="256125360"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="171988656"/>
+        <c:axId val="256859624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2629,14 +2629,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197803544"/>
+        <c:crossAx val="256125360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="197803544"/>
+        <c:axId val="256125360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2687,7 +2687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="171988656"/>
+        <c:crossAx val="256859624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3243,256 +3243,256 @@
                   <c:v>0.23500583333345004</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.24161833333346006</c:v>
+                  <c:v>0.27482916666672003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.24161833333346006</c:v>
+                  <c:v>0.27482916666672003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.24161833333346006</c:v>
+                  <c:v>0.27482916666672003</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.28209666666676003</c:v>
+                  <c:v>0.31530750000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.28209666666676003</c:v>
+                  <c:v>0.31530750000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.28475666666676003</c:v>
+                  <c:v>0.31796750000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.28475666666676003</c:v>
+                  <c:v>0.31796750000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.28475666666676003</c:v>
+                  <c:v>0.31796750000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.29856583333342002</c:v>
+                  <c:v>0.33177666666667999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.29856583333342002</c:v>
+                  <c:v>0.33177666666667999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.29856583333342002</c:v>
+                  <c:v>0.33177666666667999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.32388250000002</c:v>
+                  <c:v>0.35709333333327997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.32388250000002</c:v>
+                  <c:v>0.35709333333327997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.33244250000001002</c:v>
+                  <c:v>0.36565333333326999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.33527333333334003</c:v>
+                  <c:v>0.3684841666666</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.33527333333334003</c:v>
+                  <c:v>0.3684841666666</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.33527333333334003</c:v>
+                  <c:v>0.3684841666666</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.33527333333334003</c:v>
+                  <c:v>0.3684841666666</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.73195583333334002</c:v>
+                  <c:v>0.76516666666659994</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.73195583333334002</c:v>
+                  <c:v>0.76516666666659994</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.73195583333334002</c:v>
+                  <c:v>0.76516666666659994</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.73195583333334002</c:v>
+                  <c:v>0.76516666666659994</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.78545000000004006</c:v>
+                  <c:v>0.81866083333329998</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.78545000000004006</c:v>
+                  <c:v>0.81866083333329998</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.81003250000004001</c:v>
+                  <c:v>0.84324333333329993</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.81003250000004001</c:v>
+                  <c:v>0.84324333333329993</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.89067166666653996</c:v>
+                  <c:v>0.92388249999979988</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.91722499999994</c:v>
+                  <c:v>0.95043583333319992</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.91722499999994</c:v>
+                  <c:v>0.95043583333319992</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.97210166666660003</c:v>
+                  <c:v>0.99167083333319994</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>0.99761083333319989</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>1.0011241666665298</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>1.0011241666665298</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>1.0011241666665298</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.97804166666659997</c:v>
+                  <c:v>1.0011241666665298</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0004908333331968</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0004908333331968</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0004908333331968</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0041358333331967</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0041358333331967</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0041358333331967</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.97740833333326693</c:v>
+                  <c:v>1.0041358333331967</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.93197499999996691</c:v>
+                  <c:v>0.95870249999989665</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.93197499999996691</c:v>
+                  <c:v>0.95870249999989665</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.172604999999967</c:v>
+                  <c:v>1.1542583333331966</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.2205474999998671</c:v>
+                  <c:v>1.2022008333330967</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.2208474999998671</c:v>
+                  <c:v>1.2025008333330967</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.2208474999998671</c:v>
+                  <c:v>1.2025008333330967</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.2208474999998671</c:v>
+                  <c:v>1.2025008333330967</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.2249841666665371</c:v>
+                  <c:v>1.2066374999997667</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.2249841666665371</c:v>
+                  <c:v>1.2066374999997667</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.2249841666665371</c:v>
+                  <c:v>1.2066374999997667</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.2249841666665371</c:v>
+                  <c:v>1.2066374999997667</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.2249841666665371</c:v>
+                  <c:v>1.2066374999997667</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1.2281841666665372</c:v>
+                  <c:v>1.2098374999997668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3508,11 +3508,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="197483592"/>
-        <c:axId val="199646752"/>
+        <c:axId val="256252352"/>
+        <c:axId val="256253760"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="197483592"/>
+        <c:axId val="256252352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3555,14 +3555,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199646752"/>
+        <c:crossAx val="256253760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="199646752"/>
+        <c:axId val="256253760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,7 +3613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197483592"/>
+        <c:crossAx val="256252352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5692,7 +5692,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="F29">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A29, '1.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.11'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.21'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.10'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.22'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.11'!$A$2:$I$70,6,FALSE),0))</f>
-        <v>19.837499999999999</v>
+        <v>119.47</v>
       </c>
       <c r="G29">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A29, '1.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.11'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.21'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.10'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.22'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.11'!$A$2:$I$70,7,FALSE),0))</f>
@@ -6766,11 +6766,11 @@
       </c>
       <c r="H29">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A29, '1.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.11'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '1.21'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.10'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '2.22'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A29, '3.11'!$A$2:$I$70,8,FALSE),0))</f>
-        <v>6.6125000000100001E-3</v>
+        <v>3.9823333333269997E-2</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>0.24161833333346006</v>
+        <v>0.27482916666672003</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -6807,7 +6807,7 @@
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>0.24161833333346006</v>
+        <v>0.27482916666672003</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -6844,7 +6844,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>0.24161833333346006</v>
+        <v>0.27482916666672003</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>0.28209666666676003</v>
+        <v>0.31530750000002</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>0.28209666666676003</v>
+        <v>0.31530750000002</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -6955,7 +6955,7 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>0.28475666666676003</v>
+        <v>0.31796750000002</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -6992,7 +6992,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>0.28475666666676003</v>
+        <v>0.31796750000002</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -7029,7 +7029,7 @@
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>0.28475666666676003</v>
+        <v>0.31796750000002</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -7066,7 +7066,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>0.29856583333342002</v>
+        <v>0.33177666666667999</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>0.29856583333342002</v>
+        <v>0.33177666666667999</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -7140,7 +7140,7 @@
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>0.29856583333342002</v>
+        <v>0.33177666666667999</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -7177,7 +7177,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>0.32388250000002</v>
+        <v>0.35709333333327997</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>0.32388250000002</v>
+        <v>0.35709333333327997</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -7251,7 +7251,7 @@
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>0.33244250000001002</v>
+        <v>0.36565333333326999</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>0.33527333333334003</v>
+        <v>0.3684841666666</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -7325,7 +7325,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>0.33527333333334003</v>
+        <v>0.3684841666666</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -7362,7 +7362,7 @@
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>0.33527333333334003</v>
+        <v>0.3684841666666</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -7399,7 +7399,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>0.33527333333334003</v>
+        <v>0.3684841666666</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -7436,7 +7436,7 @@
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>0.73195583333334002</v>
+        <v>0.76516666666659994</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -7473,7 +7473,7 @@
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
-        <v>0.73195583333334002</v>
+        <v>0.76516666666659994</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -7510,7 +7510,7 @@
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>0.73195583333334002</v>
+        <v>0.76516666666659994</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -7547,7 +7547,7 @@
       </c>
       <c r="I50">
         <f t="shared" si="0"/>
-        <v>0.73195583333334002</v>
+        <v>0.76516666666659994</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
-        <v>0.78545000000004006</v>
+        <v>0.81866083333329998</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>0.78545000000004006</v>
+        <v>0.81866083333329998</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -7658,7 +7658,7 @@
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
-        <v>0.81003250000004001</v>
+        <v>0.84324333333329993</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="I54">
         <f t="shared" si="0"/>
-        <v>0.81003250000004001</v>
+        <v>0.84324333333329993</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -7732,7 +7732,7 @@
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
-        <v>0.89067166666653996</v>
+        <v>0.92388249999979988</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -7769,7 +7769,7 @@
       </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>0.91722499999994</v>
+        <v>0.95043583333319992</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="B57">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A57, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-140</v>
+        <v>-120</v>
       </c>
       <c r="C57">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A57, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -7786,7 +7786,7 @@
       </c>
       <c r="D57">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A57, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-140</v>
+        <v>-120</v>
       </c>
       <c r="E57">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A57, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A57, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
-        <v>0.91722499999994</v>
+        <v>0.95043583333319992</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -7827,7 +7827,7 @@
       </c>
       <c r="E58">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A58, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
-        <v>164.63000000000002</v>
+        <v>123.70500000000001</v>
       </c>
       <c r="F58">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A58, '1.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.11'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.21'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.10'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.22'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.11'!$A$2:$I$70,6,FALSE),0))</f>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="G58">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A58, '1.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.11'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.21'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.10'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.22'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.11'!$A$2:$I$70,7,FALSE),0))</f>
-        <v>5.4876666666660009E-2</v>
+        <v>4.1235000000000008E-2</v>
       </c>
       <c r="H58">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A58, '1.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.11'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '1.21'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.10'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '2.22'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A58, '3.11'!$A$2:$I$70,8,FALSE),0))</f>
@@ -7843,7 +7843,7 @@
       </c>
       <c r="I58">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -7880,7 +7880,7 @@
       </c>
       <c r="I59">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -7917,7 +7917,7 @@
       </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -7954,7 +7954,7 @@
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -7991,7 +7991,7 @@
       </c>
       <c r="I62">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -8028,7 +8028,7 @@
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>0.97210166666660003</v>
+        <v>0.99167083333319994</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -8139,7 +8139,7 @@
       </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -8176,7 +8176,7 @@
       </c>
       <c r="I67">
         <f t="shared" si="0"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -8213,7 +8213,7 @@
       </c>
       <c r="I68">
         <f t="shared" ref="I68:I112" si="1">SUM(G68,H68,I67)</f>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -8250,7 +8250,7 @@
       </c>
       <c r="I69">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -8287,7 +8287,7 @@
       </c>
       <c r="I70">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="B71">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A71, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C71">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A71, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8304,7 +8304,7 @@
       </c>
       <c r="D71">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A71, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="E71">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A71, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A71, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8324,7 +8324,7 @@
       </c>
       <c r="I71">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -8333,7 +8333,7 @@
       </c>
       <c r="B72">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A72, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C72">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A72, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8341,7 +8341,7 @@
       </c>
       <c r="D72">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A72, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="E72">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A72, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A72, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="I72">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>0.99761083333319989</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -8382,7 +8382,7 @@
       </c>
       <c r="E73">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A73, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
-        <v>0</v>
+        <v>10.54</v>
       </c>
       <c r="F73">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A73, '1.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.11'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.21'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.10'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.22'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.11'!$A$2:$I$70,6,FALSE),0))</f>
@@ -8390,7 +8390,7 @@
       </c>
       <c r="G73">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A73, '1.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.11'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.21'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.10'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.22'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.11'!$A$2:$I$70,7,FALSE),0))</f>
-        <v>0</v>
+        <v>3.5133333333299999E-3</v>
       </c>
       <c r="H73">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A73, '1.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.11'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '1.21'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.10'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '2.22'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A73, '3.11'!$A$2:$I$70,8,FALSE),0))</f>
@@ -8398,7 +8398,7 @@
       </c>
       <c r="I73">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>1.0011241666665298</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -8435,7 +8435,7 @@
       </c>
       <c r="I74">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>1.0011241666665298</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -8472,7 +8472,7 @@
       </c>
       <c r="I75">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>1.0011241666665298</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -8509,7 +8509,7 @@
       </c>
       <c r="I76">
         <f t="shared" si="1"/>
-        <v>0.97804166666659997</v>
+        <v>1.0011241666665298</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -8518,7 +8518,7 @@
       </c>
       <c r="B77">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A77, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-50</v>
+        <v>-40</v>
       </c>
       <c r="C77">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A77, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="D77">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A77, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-50</v>
+        <v>-40</v>
       </c>
       <c r="E77">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A77, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A77, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8546,7 +8546,7 @@
       </c>
       <c r="I77">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0004908333331968</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="B78">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A78, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="C78">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A78, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="D78">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A78, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="E78">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A78, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A78, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8583,7 +8583,7 @@
       </c>
       <c r="I78">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0004908333331968</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -8592,7 +8592,7 @@
       </c>
       <c r="B79">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A79, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="C79">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A79, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8600,7 +8600,7 @@
       </c>
       <c r="D79">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A79, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="E79">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A79, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A79, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8620,7 +8620,7 @@
       </c>
       <c r="I79">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0004908333331968</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -8629,7 +8629,7 @@
       </c>
       <c r="B80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-200</v>
+        <v>-160</v>
       </c>
       <c r="C80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8637,11 +8637,11 @@
       </c>
       <c r="D80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-200</v>
+        <v>-160</v>
       </c>
       <c r="E80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
-        <v>0</v>
+        <v>10.935</v>
       </c>
       <c r="F80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,6,FALSE),0))</f>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="G80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,7,FALSE),0))</f>
-        <v>0</v>
+        <v>3.6449999999999998E-3</v>
       </c>
       <c r="H80">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A80, '1.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.11'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '1.21'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.10'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '2.22'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A80, '3.11'!$A$2:$I$70,8,FALSE),0))</f>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="I80">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0041358333331967</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -8666,7 +8666,7 @@
       </c>
       <c r="B81">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A81, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="C81">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A81, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8674,7 +8674,7 @@
       </c>
       <c r="D81">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A81, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-200</v>
+        <v>-170</v>
       </c>
       <c r="E81">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A81, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A81, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8694,7 +8694,7 @@
       </c>
       <c r="I81">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0041358333331967</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -8703,7 +8703,7 @@
       </c>
       <c r="B82">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A82, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-400</v>
+        <v>-340</v>
       </c>
       <c r="C82">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A82, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="D82">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A82, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-400</v>
+        <v>-340</v>
       </c>
       <c r="E82">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A82, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A82, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8731,7 +8731,7 @@
       </c>
       <c r="I82">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0041358333331967</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -8740,7 +8740,7 @@
       </c>
       <c r="B83">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A83, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-800</v>
+        <v>-680</v>
       </c>
       <c r="C83">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A83, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8748,7 +8748,7 @@
       </c>
       <c r="D83">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A83, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-800</v>
+        <v>-680</v>
       </c>
       <c r="E83">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A83, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A83, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8768,7 +8768,7 @@
       </c>
       <c r="I83">
         <f t="shared" si="1"/>
-        <v>0.97740833333326693</v>
+        <v>1.0041358333331967</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -8777,7 +8777,7 @@
       </c>
       <c r="B84">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A84, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-640</v>
+        <v>-520</v>
       </c>
       <c r="C84">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A84, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8785,7 +8785,7 @@
       </c>
       <c r="D84">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A84, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-640</v>
+        <v>-520</v>
       </c>
       <c r="E84">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A84, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A84, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8805,7 +8805,7 @@
       </c>
       <c r="I84">
         <f t="shared" si="1"/>
-        <v>0.93197499999996691</v>
+        <v>0.95870249999989665</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -8814,7 +8814,7 @@
       </c>
       <c r="B85">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A85, '1.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.11'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.21'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.10'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.22'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.1'!$A$2:$I$70,2,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.11'!$A$2:$I$70,2,FALSE),0))</f>
-        <v>-640</v>
+        <v>-520</v>
       </c>
       <c r="C85">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A85, '1.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.11'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.21'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.10'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.22'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.1'!$A$2:$I$70,3,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.11'!$A$2:$I$70,3,FALSE),0))</f>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="D85">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A85, '1.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.11'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.21'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.10'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.22'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.1'!$A$2:$I$70,4,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.11'!$A$2:$I$70,4,FALSE),0))</f>
-        <v>-640</v>
+        <v>-520</v>
       </c>
       <c r="E85">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A85, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A85, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
@@ -8842,7 +8842,7 @@
       </c>
       <c r="I85">
         <f t="shared" si="1"/>
-        <v>0.93197499999996691</v>
+        <v>0.95870249999989665</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -8863,7 +8863,7 @@
       </c>
       <c r="E86">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A86, '1.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.11'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.21'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.10'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.22'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.1'!$A$2:$I$70,5,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.11'!$A$2:$I$70,5,FALSE),0))</f>
-        <v>721.89</v>
+        <v>586.66750000000002</v>
       </c>
       <c r="F86">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A86, '1.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.11'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.21'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.10'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.22'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.1'!$A$2:$I$70,6,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.11'!$A$2:$I$70,6,FALSE),0))</f>
@@ -8871,7 +8871,7 @@
       </c>
       <c r="G86">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A86, '1.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.11'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.21'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.10'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.22'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.1'!$A$2:$I$70,7,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.11'!$A$2:$I$70,7,FALSE),0))</f>
-        <v>0.24063000000000001</v>
+        <v>0.19555583333330001</v>
       </c>
       <c r="H86">
         <f>SUM(_xlfn.IFNA(VLOOKUP(A86, '1.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.11'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '1.21'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.10'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '2.22'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.1'!$A$2:$I$70,8,FALSE),0), _xlfn.IFNA(VLOOKUP(A86, '3.11'!$A$2:$I$70,8,FALSE),0))</f>
@@ -8879,7 +8879,7 @@
       </c>
       <c r="I86">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -8916,7 +8916,7 @@
       </c>
       <c r="I87">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -8953,7 +8953,7 @@
       </c>
       <c r="I88">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -8990,7 +8990,7 @@
       </c>
       <c r="I89">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -9027,7 +9027,7 @@
       </c>
       <c r="I90">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -9064,7 +9064,7 @@
       </c>
       <c r="I91">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -9101,7 +9101,7 @@
       </c>
       <c r="I92">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -9138,7 +9138,7 @@
       </c>
       <c r="I93">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -9175,7 +9175,7 @@
       </c>
       <c r="I94">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -9212,7 +9212,7 @@
       </c>
       <c r="I95">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -9249,7 +9249,7 @@
       </c>
       <c r="I96">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -9286,7 +9286,7 @@
       </c>
       <c r="I97">
         <f t="shared" si="1"/>
-        <v>1.172604999999967</v>
+        <v>1.1542583333331966</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="I98">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -9360,7 +9360,7 @@
       </c>
       <c r="I99">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -9397,7 +9397,7 @@
       </c>
       <c r="I100">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -9434,7 +9434,7 @@
       </c>
       <c r="I101">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -9471,7 +9471,7 @@
       </c>
       <c r="I102">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -9508,7 +9508,7 @@
       </c>
       <c r="I103">
         <f t="shared" si="1"/>
-        <v>1.2205474999998671</v>
+        <v>1.2022008333330967</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -9545,7 +9545,7 @@
       </c>
       <c r="I104">
         <f t="shared" si="1"/>
-        <v>1.2208474999998671</v>
+        <v>1.2025008333330967</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -9582,7 +9582,7 @@
       </c>
       <c r="I105">
         <f t="shared" si="1"/>
-        <v>1.2208474999998671</v>
+        <v>1.2025008333330967</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -9619,7 +9619,7 @@
       </c>
       <c r="I106">
         <f t="shared" si="1"/>
-        <v>1.2208474999998671</v>
+        <v>1.2025008333330967</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -9656,7 +9656,7 @@
       </c>
       <c r="I107">
         <f t="shared" si="1"/>
-        <v>1.2249841666665371</v>
+        <v>1.2066374999997667</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="I108">
         <f t="shared" si="1"/>
-        <v>1.2249841666665371</v>
+        <v>1.2066374999997667</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -9730,7 +9730,7 @@
       </c>
       <c r="I109">
         <f t="shared" si="1"/>
-        <v>1.2249841666665371</v>
+        <v>1.2066374999997667</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -9767,7 +9767,7 @@
       </c>
       <c r="I110">
         <f t="shared" si="1"/>
-        <v>1.2249841666665371</v>
+        <v>1.2066374999997667</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -9804,7 +9804,7 @@
       </c>
       <c r="I111">
         <f t="shared" si="1"/>
-        <v>1.2249841666665371</v>
+        <v>1.2066374999997667</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="I112">
         <f t="shared" si="1"/>
-        <v>1.2281841666665372</v>
+        <v>1.2098374999997668</v>
       </c>
     </row>
   </sheetData>
@@ -9854,8 +9854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10881,13 +10881,13 @@
         <v>42451.704861111109</v>
       </c>
       <c r="B57">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="I57">
         <v>0.129075</v>
@@ -10906,14 +10906,8 @@
       <c r="D58">
         <v>0</v>
       </c>
-      <c r="E58">
-        <v>20.462499999999999</v>
-      </c>
-      <c r="G58">
-        <v>6.82083333333E-3</v>
-      </c>
       <c r="I58">
-        <v>0.13589583333300001</v>
+        <v>0.129075</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -10930,7 +10924,7 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>0.13589583333300001</v>
+        <v>0.129075</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -10947,7 +10941,7 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <v>0.13589583333300001</v>
+        <v>0.129075</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -10964,7 +10958,7 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>0.13589583333300001</v>
+        <v>0.129075</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -10981,7 +10975,7 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>0.13589583333300001</v>
+        <v>0.129075</v>
       </c>
     </row>
   </sheetData>
@@ -10994,7 +10988,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12154,7 +12148,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12480,10 +12474,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>6.6124999999999998</v>
+        <v>46.51</v>
       </c>
       <c r="H16">
-        <v>2.20416666667E-3</v>
+        <v>1.55033333333E-2</v>
       </c>
       <c r="I16">
         <v>5.80841666667E-2</v>
@@ -13339,7 +13333,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection sqref="A1:I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13535,10 +13529,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>6.6124999999999998</v>
+        <v>46.51</v>
       </c>
       <c r="H9">
-        <v>2.20416666667E-3</v>
+        <v>1.55033333333E-2</v>
       </c>
       <c r="I9">
         <v>5.4427499999999997E-2</v>
@@ -14525,7 +14519,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14584,10 +14578,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>6.6124999999999998</v>
+        <v>26.45</v>
       </c>
       <c r="H2">
-        <v>2.20416666667E-3</v>
+        <v>8.8166666666699995E-3</v>
       </c>
       <c r="I2">
         <v>8.8166666666699995E-3</v>
@@ -15694,7 +15688,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection sqref="A1:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16851,7 +16845,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection sqref="A1:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17156,13 +17150,13 @@
         <v>42451.704861111109</v>
       </c>
       <c r="B16">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>6.6381666666700007E-2</v>
@@ -17181,14 +17175,8 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17">
-        <v>20.462499999999999</v>
-      </c>
-      <c r="G17">
-        <v>6.82083333333E-3</v>
-      </c>
       <c r="I17">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -17205,7 +17193,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -17222,7 +17210,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -17239,7 +17227,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -17256,7 +17244,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -17273,7 +17261,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -17290,7 +17278,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -17307,7 +17295,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -17324,7 +17312,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -17341,7 +17329,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -17358,7 +17346,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -17375,7 +17363,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -17392,7 +17380,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -17400,16 +17388,16 @@
         <v>42472.704861111109</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I30">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -17417,16 +17405,16 @@
         <v>42473.704861111109</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I31">
-        <v>7.3202500000000004E-2</v>
+        <v>6.6381666666700007E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -17442,8 +17430,14 @@
       <c r="D32">
         <v>0</v>
       </c>
+      <c r="E32">
+        <v>10.54</v>
+      </c>
+      <c r="G32">
+        <v>3.5133333333299999E-3</v>
+      </c>
       <c r="I32">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -17460,7 +17454,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -17477,7 +17471,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -17494,7 +17488,7 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -17502,16 +17496,16 @@
         <v>42480.600694444445</v>
       </c>
       <c r="B36">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -17519,16 +17513,16 @@
         <v>42481.704861111109</v>
       </c>
       <c r="B37">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="I37">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -17536,16 +17530,16 @@
         <v>42482.704861111109</v>
       </c>
       <c r="B38">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="I38">
-        <v>7.3202500000000004E-2</v>
+        <v>6.9894999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -17553,16 +17547,22 @@
         <v>42485.704861111109</v>
       </c>
       <c r="B39">
-        <v>-40</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>-40</v>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>10.935</v>
+      </c>
+      <c r="G39">
+        <v>3.6449999999999998E-3</v>
       </c>
       <c r="I39">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -17570,16 +17570,16 @@
         <v>42486.704861111109</v>
       </c>
       <c r="B40">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="I40">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -17587,16 +17587,16 @@
         <v>42487.704861111109</v>
       </c>
       <c r="B41">
-        <v>-80</v>
+        <v>-20</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>-80</v>
+        <v>-20</v>
       </c>
       <c r="I41">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -17604,16 +17604,16 @@
         <v>42488.704861111109</v>
       </c>
       <c r="B42">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="I42">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -17621,16 +17621,16 @@
         <v>42489.704861111109</v>
       </c>
       <c r="B43">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="I43">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -17638,16 +17638,16 @@
         <v>42492.704861111109</v>
       </c>
       <c r="B44">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>-160</v>
+        <v>-40</v>
       </c>
       <c r="I44">
-        <v>7.3202500000000004E-2</v>
+        <v>7.3539999999999994E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -17664,13 +17664,13 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>180.4725</v>
+        <v>45.25</v>
       </c>
       <c r="G45">
-        <v>6.0157500000000003E-2</v>
+        <v>1.50833333333E-2</v>
       </c>
       <c r="I45">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -17687,7 +17687,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -17704,7 +17704,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -17721,7 +17721,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -17738,7 +17738,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -17755,7 +17755,7 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -17772,7 +17772,7 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -17789,7 +17789,7 @@
         <v>-10</v>
       </c>
       <c r="I52">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -17806,7 +17806,7 @@
         <v>-10</v>
       </c>
       <c r="I53">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -17823,7 +17823,7 @@
         <v>-20</v>
       </c>
       <c r="I54">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -17840,7 +17840,7 @@
         <v>-40</v>
       </c>
       <c r="I55">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -17857,7 +17857,7 @@
         <v>-40</v>
       </c>
       <c r="I56">
-        <v>0.13336000000000001</v>
+        <v>8.8623333333299997E-2</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -17880,7 +17880,7 @@
         <v>1.5980833333299999E-2</v>
       </c>
       <c r="I57">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -17897,7 +17897,7 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -17914,7 +17914,7 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -17931,7 +17931,7 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -17948,7 +17948,7 @@
         <v>-10</v>
       </c>
       <c r="I61">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -17965,7 +17965,7 @@
         <v>-10</v>
       </c>
       <c r="I62">
-        <v>0.14934083333299999</v>
+        <v>0.104604166667</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -17988,7 +17988,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="I63">
-        <v>0.14964083333299999</v>
+        <v>0.104904166667</v>
       </c>
     </row>
   </sheetData>
@@ -18000,8 +18000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>